<commit_message>
添加了发送web文件的部分 Signed-off-by: leafspace <leafspace_zhang@163.com>
</commit_message>
<xml_diff>
--- a/程序代码/功能VerUP列表.xlsx
+++ b/程序代码/功能VerUP列表.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1"/>
@@ -36,6 +39,163 @@
   <si>
     <t>做成人</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>严重程度</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>★★★★☆</t>
+  </si>
+  <si>
+    <t>★★★★★</t>
+  </si>
+  <si>
+    <t>★★★★★</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>★★★★☆</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>★★★☆☆</t>
+  </si>
+  <si>
+    <t>★★★☆☆</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>★★☆☆☆</t>
+  </si>
+  <si>
+    <t>★★☆☆☆</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>★☆☆☆☆</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>USB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>转串口通讯存在问题，程序无法正常接收到数据</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>监听数据与发送MFC操作请求多线程操作</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>动态做成MFC操作数据还未搭建</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>远程设置MFCIP地址与相关设置</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>树</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>莓派接收</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>请</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>求返回做成文件数据</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>远程监控树莓派端日志数据</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>搭建web服</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>务器发送给</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MFC文件</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>张立飞</t>
+  </si>
+  <si>
+    <t>张立飞</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>夏博</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>池媚媚</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>卢兵</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>夏博</t>
   </si>
 </sst>
 </file>
@@ -101,10 +261,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -406,730 +567,1118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="76.375" customWidth="1"/>
+    <col min="3" max="3" width="11.25" customWidth="1"/>
+    <col min="8" max="8" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="1"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="1"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="1"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="1"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="1"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="1"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="1"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="1"/>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="1"/>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="1"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="1"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="1"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="1"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="1"/>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="1"/>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A53" s="1"/>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A54" s="1"/>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A55" s="1"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="1"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="1"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A58" s="1"/>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A59" s="1"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="1"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A61" s="1"/>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A62" s="1"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A63" s="1"/>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A64" s="1"/>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" s="1"/>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" s="1"/>
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" s="1"/>
+      <c r="F66" s="1"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="1"/>
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="1"/>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" s="1"/>
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A71" s="1"/>
+      <c r="F70" s="1"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A72" s="1"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A73" s="1"/>
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A74" s="1"/>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="1"/>
+      <c r="F74" s="1"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A76" s="1"/>
+      <c r="F75" s="1"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A77" s="1"/>
+      <c r="F76" s="1"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A78" s="1"/>
+      <c r="F77" s="1"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="1"/>
+      <c r="F78" s="1"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A80" s="1"/>
+      <c r="F79" s="1"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A81" s="1"/>
+      <c r="F80" s="1"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A82" s="1"/>
+      <c r="F81" s="1"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A83" s="1"/>
+      <c r="F82" s="1"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A84" s="1"/>
+      <c r="F83" s="1"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A85" s="1"/>
+      <c r="F84" s="1"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A86" s="1"/>
+      <c r="F85" s="1"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A87" s="1"/>
+      <c r="F86" s="1"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A88" s="1"/>
+      <c r="F87" s="1"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A89" s="1"/>
+      <c r="F88" s="1"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A90" s="1"/>
+      <c r="F89" s="1"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A91" s="1"/>
+      <c r="F90" s="1"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A92" s="1"/>
+      <c r="F91" s="1"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A93" s="1"/>
+      <c r="F92" s="1"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A94" s="1"/>
+      <c r="F93" s="1"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A95" s="1"/>
+      <c r="F94" s="1"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A96" s="1"/>
+      <c r="F95" s="1"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A97" s="1"/>
+      <c r="F96" s="1"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A98" s="1"/>
+      <c r="F97" s="1"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A99" s="1"/>
+      <c r="F98" s="1"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A100" s="1"/>
+      <c r="F99" s="1"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1"/>
   <phoneticPr fontId="1"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C100">
+      <formula1>$H$2:$H$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:F100">
+      <formula1>$I$2:$I$5</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Finishi the web server Signed-off-by: leafspace <leafspace_zhang@163.com>
</commit_message>
<xml_diff>
--- a/程序代码/功能VerUP列表.xlsx
+++ b/程序代码/功能VerUP列表.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1"/>
@@ -571,7 +571,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -643,7 +643,9 @@
       <c r="E3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
@@ -664,7 +666,9 @@
       <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="H4" s="1" t="s">
         <v>11</v>
@@ -689,7 +693,9 @@
       <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
@@ -710,7 +716,9 @@
       <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="H6" s="1" t="s">
         <v>14</v>
@@ -729,8 +737,12 @@
       <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="1">

</xml_diff>

<commit_message>
Finishi the most function Signed-off-by: leafspace <leafspace_zhang@163.com>
</commit_message>
<xml_diff>
--- a/程序代码/功能VerUP列表.xlsx
+++ b/程序代码/功能VerUP列表.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1"/>
@@ -571,7 +571,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -669,7 +669,9 @@
       <c r="E4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>